<commit_message>
MATLAB Finding real world length per pixel given depth information
</commit_message>
<xml_diff>
--- a/Data/michaelDataCollection.xlsx
+++ b/Data/michaelDataCollection.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Senior-Design\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,8 +102,918 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2450</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9FD0-4DA3-BD51-83BB127055E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="386487328"/>
+        <c:axId val="386493560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="386487328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="386493560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="386493560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="386487328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,7 +1059,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -177,9 +1092,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,6 +1144,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -391,19 +1340,19 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -411,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -428,7 +1377,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -445,7 +1394,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -462,7 +1411,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7</v>
       </c>
@@ -479,7 +1428,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -496,7 +1445,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -513,7 +1462,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -530,7 +1479,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -544,6 +1493,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -553,7 +1503,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -565,7 +1515,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates from last commit, new project
</commit_message>
<xml_diff>
--- a/Data/michaelDataCollection.xlsx
+++ b/Data/michaelDataCollection.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -184,6 +184,64 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$8</c:f>
@@ -425,7 +483,427 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.0610673665791773E-2"/>
+                  <c:y val="-2.6246719160104987E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$16:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2450</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD53-4ED8-8EC3-CD336A40AC83}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="477887928"/>
+        <c:axId val="471095096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="477887928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="471095096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="471095096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="477887928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -981,24 +1459,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1008,6 +2008,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70AC1B07-ADD8-48AD-80C5-CFE75734ECB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1337,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,6 +2524,54 @@
       </c>
       <c r="E13" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1650</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1800</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2100</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2450</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2700</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3000</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>